<commit_message>
comprehend and feed extract
</commit_message>
<xml_diff>
--- a/rss_feed.xlsx
+++ b/rss_feed.xlsx
@@ -8,20 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Deepali_Notes\AWS_Course\news_rss_feed_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42489926-EB8A-4DCA-BD03-6ED6A374934F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1447F8BD-69C2-46FC-9D8B-4FC2DFDFA73E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirement" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
+    <sheet name="Table1" sheetId="4" r:id="rId3"/>
+    <sheet name="Table2" sheetId="5" r:id="rId4"/>
+    <sheet name="Table3" sheetId="6" r:id="rId5"/>
+    <sheet name="RDS- Postgres DB " sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="85">
   <si>
     <r>
       <rPr>
@@ -267,6 +271,102 @@
   </si>
   <si>
     <t>(for suggestions on syntax in pycharm)</t>
+  </si>
+  <si>
+    <t>News_Origin</t>
+  </si>
+  <si>
+    <t>News_URL</t>
+  </si>
+  <si>
+    <t>Active_Flag</t>
+  </si>
+  <si>
+    <t>TOI</t>
+  </si>
+  <si>
+    <t>https://timesofindia.indiatimes.com/</t>
+  </si>
+  <si>
+    <t>BS</t>
+  </si>
+  <si>
+    <t>https://www.business-standard.com/</t>
+  </si>
+  <si>
+    <t>https://timesofindia.indiatimes.com/rss.cms</t>
+  </si>
+  <si>
+    <t>RSS_List</t>
+  </si>
+  <si>
+    <t>https://www.business-standard.com/rss-feeds/listing/</t>
+  </si>
+  <si>
+    <t>https://www.hindustantimes.com/rss</t>
+  </si>
+  <si>
+    <t>https://www.hindustantimes.com/</t>
+  </si>
+  <si>
+    <t>HT</t>
+  </si>
+  <si>
+    <t>NDTV</t>
+  </si>
+  <si>
+    <t>https://www.ndtv.com/rss</t>
+  </si>
+  <si>
+    <t>https://www.ndtv.com/</t>
+  </si>
+  <si>
+    <t>RSS_Feed</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Body</t>
+  </si>
+  <si>
+    <t>Publish_Date</t>
+  </si>
+  <si>
+    <t>Sentiment</t>
+  </si>
+  <si>
+    <t>Updated_Time_Stamp</t>
+  </si>
+  <si>
+    <t>Inserted_Time_Stamp</t>
+  </si>
+  <si>
+    <t>AWS postgres DB Details:-</t>
+  </si>
+  <si>
+    <t>DB identifier: postgres-db-identifier1</t>
+  </si>
+  <si>
+    <t>master user name: postgres_admin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">password: postgres123 </t>
+  </si>
+  <si>
+    <t>Database port : 5432</t>
+  </si>
+  <si>
+    <t>KMS key ID</t>
+  </si>
+  <si>
+    <t>d5f76173-6e42-4fae-94fd-e6b8bd9bdc7d</t>
+  </si>
+  <si>
+    <t>DATABASE NAME: db_news_feed</t>
   </si>
 </sst>
 </file>
@@ -906,7 +1006,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -975,6 +1075,7 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="42"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1382,7 +1483,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:M57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
@@ -1759,4 +1860,228 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F72EAFD5-EAAC-4BA8-AAC0-F2D42E0597EE}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{E8C90861-6EE2-42DC-BA3C-CBC43D490772}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{7ED973F0-D10B-4980-B5F2-D2EB76D313CF}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{73C40F5D-69CA-40A0-9439-B1417CD35A55}"/>
+    <hyperlink ref="C4" r:id="rId4" xr:uid="{BA5376DD-782F-4E6F-A992-AA3FF5025AB2}"/>
+    <hyperlink ref="B5" r:id="rId5" xr:uid="{461D2FA7-8B06-4E4F-A076-82EC107CC537}"/>
+    <hyperlink ref="C5" r:id="rId6" xr:uid="{C5987122-2181-4F7C-9E6D-9A51300900B7}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83AF10F8-EE80-4E3F-8253-FBD0FE6087CA}">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D263AC35-2D34-4A5F-96AB-61A67799974B}">
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63D4A617-D9EC-486D-AC24-9945D152E8FD}">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>